<commit_message>
Differentiate age vs. grade scripts
</commit_message>
<xml_diff>
--- a/INPUT-FILES/NORMS/TODE_8.27.21_fornorms/TOD-E demographic variable labels.xlsx
+++ b/INPUT-FILES/NORMS/TODE_8.27.21_fornorms/TOD-E demographic variable labels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dherzberg/Desktop/R/TOD-R/INPUT-FILES/NORMS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dherzberg/Desktop/R/TOD-R/INPUT-FILES/NORMS/TODE_8.27.21_fornorms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179A4929-1ACA-F744-AB4C-E74F53AECBE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6AF102-CC08-DE4D-8B7B-083C304A1B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4C924A35-86B4-4486-8783-609F2044D53F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{4C924A35-86B4-4486-8783-609F2044D53F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Gender</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>*in the census, American Indian and Native Hawaiian are included with "Other"</t>
+  </si>
+  <si>
+    <t>option for cNORM recoding, express grade as weeks in school</t>
   </si>
 </sst>
 </file>
@@ -546,8 +549,8 @@
   </sheetPr>
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -744,7 +747,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -752,7 +755,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -760,7 +763,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>5</v>
       </c>
@@ -768,7 +771,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>6</v>
       </c>
@@ -776,7 +779,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>7</v>
       </c>
@@ -784,7 +787,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>8</v>
       </c>
@@ -792,57 +795,78 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
       <c r="B41" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2</v>
       </c>
       <c r="B42" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3</v>
       </c>
       <c r="B43" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>4</v>
       </c>
       <c r="B44" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>5</v>
       </c>
       <c r="B45" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>6</v>
       </c>
       <c r="B46" t="s">
         <v>37</v>
+      </c>
+      <c r="C46">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>